<commit_message>
Add name to Analysis
</commit_message>
<xml_diff>
--- a/project/excel/ars_ldm.xlsx
+++ b/project/excel/ars_ldm.xlsx
@@ -480,66 +480,71 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>categoryIds</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>analysisSetId</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>orderedGroupings</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>dataSubsetId</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>dataset</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>variable</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>methodId</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>referencedAnalysisOperations</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>results</t>
         </is>
@@ -1710,66 +1715,71 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>categoryIds</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>analysisSetId</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>orderedGroupings</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>dataSubsetId</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>dataset</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>variable</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>methodId</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>referencedAnalysisOperations</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>results</t>
         </is>

</xml_diff>

<commit_message>
Sprint 12 - comparative stats
</commit_message>
<xml_diff>
--- a/project/excel/ars_ldm.xlsx
+++ b/project/excel/ars_ldm.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="67" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="67" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" state="visible" r:id="rId1"/>
@@ -111,15 +111,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -551,7 +551,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -582,7 +582,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -624,14 +624,14 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C1048576" type="list">
+    <dataValidation sqref="C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"EQ,NE,GT,GE,LT,LE,IN,NOTIN"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C1048576" type="list">
+    <dataValidation sqref="C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"EQ,NE,GT,GE,LT,LE,IN,NOTIN"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -682,7 +682,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -728,7 +728,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -779,7 +779,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -825,7 +825,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -857,14 +857,14 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2:A1048576" type="list">
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Title,Footnote,Abbreviation,Legend,Rowlabel Header"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2:A1048576" type="list">
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"Title,Footnote,Abbreviation,Legend,Rowlabel Header"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -900,7 +900,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -942,14 +942,14 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B1048576" type="list">
+    <dataValidation sqref="B2:B1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"pdf,rtf,txt"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B1048576" type="list">
+    <dataValidation sqref="B2:B1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"pdf,rtf,txt"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1000,7 +1000,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1036,7 +1036,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1082,7 +1082,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1108,7 +1108,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1134,7 +1134,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1180,7 +1180,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1221,7 +1221,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1231,6 +1231,206 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>OrderedGroupingFactor_order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>groupingId</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dataGrouping</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>resultsByGroup</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>OrderedListItem_level</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>OrderedListItem_order</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sublist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>analysisId</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>outputId</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fileSpecifications</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>outputDisplays</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Output_categoryIds</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>OutputDisplay_order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>display</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>referencedOperationId</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ReferencedAnalysisOperation_analysisId</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1242,271 +1442,76 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OrderedGroupingFactor_order</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>groupingId</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>dataGrouping</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>OrderedListItem_level</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrderedListItem_order</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sublist</t>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>subCategorizations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>referencedOperationRole</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>operationId</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>analysisId</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>analysisId</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>outputId</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>fileSpecifications</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>outputDisplays</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Output_categoryIds</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>OutputDisplay_order</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>display</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>referencedOperationId</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ReferencedAnalysisOperation_analysisId</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>subCategorizations</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>referencedOperationRole</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>operationId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>analysisId</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B1048576" type="list">
+    <dataValidation sqref="B2:B1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"NUMERATOR,DENOMINATOR"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B1048576" type="list">
+    <dataValidation sqref="B2:B1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"NUMERATOR,DENOMINATOR"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1582,7 +1587,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1618,7 +1623,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1664,7 +1669,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1705,7 +1710,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1786,7 +1791,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1822,7 +1827,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1858,7 +1863,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1909,7 +1914,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1955,7 +1960,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2006,7 +2011,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2057,7 +2062,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2088,7 +2093,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2119,7 +2124,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2150,7 +2155,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2181,7 +2186,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2222,7 +2227,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2273,7 +2278,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2319,7 +2324,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2370,7 +2375,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2416,7 +2421,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2462,7 +2467,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2493,7 +2498,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2529,7 +2534,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2570,7 +2575,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2621,7 +2626,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2667,7 +2672,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2693,7 +2698,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2719,7 +2724,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2765,7 +2770,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2806,7 +2811,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2816,6 +2821,379 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>OrderedGroupingFactor_order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>groupingId</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dataGrouping</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>resultsByGroup</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>condition</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>AnalysisSet_compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>OrderedListItem_level</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>OrderedListItem_order</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sublist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>analysisId</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>outputId</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fileSpecifications</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>outputDisplays</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Output_categoryIds</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>OutputDisplay_order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>display</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>referencedOperationId</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ReferencedAnalysisOperation_analysisId</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>referencedOperationRole</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>operationId</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>analysisId</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>listOfPlannedAnalyses</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>listOfPlannedOutputs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>analysisSets</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>analysisGroupings</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dataSubsets</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>globalDisplaySections</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>analysisCategorizations</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>analyses</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>methods</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2827,32 +3205,78 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OrderedGroupingFactor_order</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>groupingId</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>dataGrouping</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>groupId</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>groupValue</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>groupingVariable</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dataDriven</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>SubjectGroupingFactor_groups</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2878,123 +3302,16 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>AnalysisSet_compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>OrderedListItem_level</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrderedListItem_order</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sublist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>analysisId</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>outputId</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>fileSpecifications</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>outputDisplays</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Output_categoryIds</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3011,313 +3328,6 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OutputDisplay_order</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>display</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>referencedOperationId</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ReferencedAnalysisOperation_analysisId</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>referencedOperationRole</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>operationId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>analysisId</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>listOfPlannedAnalyses</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>listOfPlannedOutputs</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>analysisSets</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>analysisGroupings</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>dataSubsets</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>globalDisplaySections</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>analysisCategorizations</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>analyses</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>methods</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>outputs</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>groupingId</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>groupId</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>groupValue</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>groupingVariable</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>dataDriven</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>SubjectGroupingFactor_groups</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>logicalOperator</t>
         </is>
       </c>
@@ -3329,14 +3339,14 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2:A1048576" type="list">
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"AND,OR,NOT"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2:A1048576" type="list">
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"AND,OR,NOT"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -3367,7 +3377,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -3398,6 +3408,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ARM elements and documentation updates
</commit_message>
<xml_diff>
--- a/project/excel/ars_ldm.xlsx
+++ b/project/excel/ars_ldm.xlsx
@@ -20,38 +20,40 @@
     <sheet name="AnalysisMethod" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Operation" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="ReferencedOperationRelationship" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="ProgrammingCodeTemplate" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="CodeParameter" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Output" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="File" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="OrderedDisplay" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="OutputDisplay" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="DisplaySection" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="DisplaySubSection" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="WhereClause" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="WhereClauseCondition" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="WhereClauseCompoundExpression" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="CompoundSetExpression" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="CompoundGroupExpression" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="CompoundSubsetExpression" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="AnalysisSet" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="SubjectGroupingFactor" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="DataGroupingFactor" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="Group" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="AnalysisGroup" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="DataGroup" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="DataSubset" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="ReferenceDocument" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="DocumentRef" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="PageRef" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="PageNumberListRef" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="PageNumberRangeRef" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="PageNameRef" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="PageNumberList" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="PageNameList" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="PageRange" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="TerminologyExtension" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="SponsorTerm" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="AnalysisOutputProgrammingCode" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AnalysisProgrammingCodeTemplate" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="CodeParameter" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="TemplateCodeParameter" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Output" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="OutputFile" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="OrderedDisplay" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="OutputDisplay" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="DisplaySection" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="DisplaySubSection" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="WhereClause" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="WhereClauseCondition" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="WhereClauseCompoundExpression" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="CompoundSetExpression" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="CompoundGroupExpression" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="CompoundSubsetExpression" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="AnalysisSet" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="SubjectGroupingFactor" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="DataGroupingFactor" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Group" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="AnalysisGroup" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="DataGroup" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="DataSubset" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="ReferenceDocument" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="DocumentRef" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="PageRef" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="PageNumberListRef" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="PageNumberRangeRef" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="PageNameRef" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="PageNumberList" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="PageNameList" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="PageRange" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="TerminologyExtension" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="SponsorTerm" sheetId="47" state="visible" r:id="rId47"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -584,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,11 +617,328 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>documentRefs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>codeTemplate</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>referencedOperationRelationships</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>resultPattern</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>referencedOperationRole</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>operationId</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>analysisId</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>context</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>documentRefs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>parameters</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>context</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>documentRefs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>parameters</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>valueSource</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fileSpecifications</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>displays</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>categoryIds</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>documentRefs</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>programmingCode</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
@@ -629,7 +948,105 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>fileType</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>style</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>listItems</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>display</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -651,17 +1068,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>referencedOperationRelationships</t>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>displayTitle</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>resultPattern</t>
+          <t>displaySections</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -675,315 +1092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>referencedOperationRole</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>operationId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>analysisId</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>context</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>parameters</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>templateCode</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>valueSource</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>fileSpecifications</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>displays</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>categoryIds</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>fileType</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>style</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>display</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>displayTitle</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>displaySections</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>listItems</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1019,7 +1128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1055,7 +1164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1096,7 +1205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1142,7 +1251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1178,7 +1287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1214,7 +1323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1250,7 +1359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1286,7 +1395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1303,6 +1412,57 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sublist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>analysisId</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>outputId</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1337,7 +1497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1383,7 +1543,53 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>groupingVariable</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dataDriven</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>groups</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1400,31 +1606,220 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>level</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>order</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>sublist</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>condition</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>level</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>analysisId</t>
+          <t>order</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>outputId</t>
+          <t>condition</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>condition</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>condition</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
@@ -1434,293 +1829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>groupingVariable</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>dataDriven</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>groups</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1751,7 +1860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1792,7 +1901,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1833,7 +1978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1874,43 +2019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>categories</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1951,7 +2060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1977,7 +2086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2003,7 +2112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2034,7 +2143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2070,7 +2179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2148,7 +2257,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2179,19 +2288,19 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>reason</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>documentRefs</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>reason</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>purpose</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
         <is>
           <t>analysisSetId</t>
@@ -2229,10 +2338,15 @@
       </c>
       <c r="O1" t="inlineStr">
         <is>
+          <t>programmingCode</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
           <t>results</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>name</t>
         </is>

</xml_diff>

<commit_message>
Issue 205 and reorder slots in OrderedListItem
</commit_message>
<xml_diff>
--- a/project/excel/ars_ldm.xlsx
+++ b/project/excel/ars_ldm.xlsx
@@ -13,8 +13,8 @@
     <sheet name="ReferenceDocument" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="TerminologyExtension" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="SponsorTerm" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="AnalysisCategorization" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AnalysisCategory" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AnalysisOutputCategorization" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="AnalysisOutputCategory" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="WhereClause" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="WhereClauseCondition" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="WhereClauseCompoundExpression" sheetId="11" state="visible" r:id="rId11"/>
@@ -507,7 +507,7 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>analysisCategorizations</t>
+          <t>analysisOutputCategorizations</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -1534,17 +1534,17 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>analysisId</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>outputId</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>sublist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>analysisId</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>outputId</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">

</xml_diff>

<commit_message>
Model updates for ARSP-17, #187, #200, #208, #210, #217
</commit_message>
<xml_diff>
--- a/project/excel/ars_ldm.xlsx
+++ b/project/excel/ars_ldm.xlsx
@@ -8,59 +8,60 @@
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NestedList" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="OrderedListItem" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ReferenceDocument" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="TerminologyExtension" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="SponsorTerm" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="AnalysisOutputCategorization" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AnalysisOutputCategory" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="WhereClause" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="WhereClauseCondition" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="WhereClauseCompoundExpression" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="AnalysisSet" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="CompoundSetExpression" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="DataSubset" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="CompoundSubsetExpression" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Group" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="CompoundGroupExpression" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="SubjectGroupingFactor" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="AnalysisGroup" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="DataGroupingFactor" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="DataGroup" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="AnalysisMethod" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="DocumentReference" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="PageNumberListRef" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="PageNumberRangeRef" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="PageNameRef" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="Operation" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="ReferencedOperationRelationship" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="OperationRole" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="SponsorOperationRole" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="AnalysisProgrammingCodeTemplate" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="TemplateCodeParameter" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="Analysis" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="AnalysisReason" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="SponsorAnalysisReason" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="AnalysisPurpose" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="SponsorAnalysisPurpose" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="OrderedGroupingFactor" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="ReferencedAnalysisOperation" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="AnalysisOutputProgrammingCode" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="AnalysisOutputCodeParameter" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="OperationResult" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="ResultGroup" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="GlobalDisplaySection" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="DisplaySubSection" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="Output" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="OutputFile" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet name="OutputFileType" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet name="SponsorOutputFileType" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet name="OrderedDisplay" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet name="OutputDisplay" sheetId="51" state="visible" r:id="rId51"/>
-    <sheet name="DisplaySection" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet name="OrderedSubSection" sheetId="53" state="visible" r:id="rId53"/>
-    <sheet name="OrderedSubSectionRef" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet name="ListOfContents" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NestedList" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="OrderedListItem" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ReferenceDocument" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TerminologyExtension" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SponsorTerm" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="AnalysisOutputCategorization" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="AnalysisOutputCategory" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="WhereClause" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="WhereClauseCondition" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="WhereClauseCompoundExpression" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="AnalysisSet" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="CompoundSetExpression" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="DataSubset" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="CompoundSubsetExpression" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Group" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="CompoundGroupExpression" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="SubjectGroupingFactor" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="AnalysisGroup" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="DataGroupingFactor" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="DataGroup" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="AnalysisMethod" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="DocumentReference" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="PageNumberListRef" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="PageNumberRangeRef" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="PageNameRef" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Operation" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="ReferencedOperationRelationship" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="OperationRole" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="SponsorOperationRole" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="AnalysisProgrammingCodeTemplate" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="TemplateCodeParameter" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="Analysis" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="AnalysisReason" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="SponsorAnalysisReason" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="AnalysisPurpose" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="SponsorAnalysisPurpose" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="OrderedGroupingFactor" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="ReferencedAnalysisOperation" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="AnalysisOutputProgrammingCode" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="AnalysisOutputCodeParameter" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="OperationResult" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="ResultGroup" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="GlobalDisplaySection" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="DisplaySubSection" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="Output" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="OutputFile" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="OutputFileType" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="SponsorOutputFileType" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="OrderedDisplay" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="OutputDisplay" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet name="DisplaySection" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet name="OrderedSubSection" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet name="OrderedSubSectionRef" sheetId="55" state="visible" r:id="rId55"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,12 +488,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>listOfPlannedAnalyses</t>
+          <t>mainListOfContents</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>listOfPlannedOutputs</t>
+          <t>otherListsOfContents</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -555,6 +556,16 @@
           <t>name</t>
         </is>
       </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -562,6 +573,47 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>condition</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -607,7 +659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -643,7 +695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -694,7 +746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -730,7 +782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -781,7 +833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -817,7 +869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -868,7 +920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -904,13 +956,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -931,32 +983,231 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>groupingDataset</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>groupingVariable</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dataDriven</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>groups</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>contentsList</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>condition</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>groupingDataset</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>groupingVariable</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>dataDriven</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>groups</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>groups</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
+          <t>condition</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>compoundExpression</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -972,215 +1223,41 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>documentRefs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>operations</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>codeTemplate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>label</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>listItems</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>groupingVariable</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>dataDriven</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>groups</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>documentRefs</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>operations</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>codeTemplate</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1211,7 +1288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1267,7 +1344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1323,7 +1400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1379,7 +1456,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>referencedOperationRelationships</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>resultPattern</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1401,67 +1534,21 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>referencedOperationRelationships</t>
+          <t>referencedOperationRole</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>operationId</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>resultPattern</t>
+          <t>analysisId</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>referencedOperationRole</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>operationId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>analysisId</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
           <t>description</t>
         </is>
       </c>
@@ -1471,7 +1558,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>listItems</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1507,277 +1620,236 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>analysisId</t>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>controlledTerm</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sponsorTermId</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>context</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>documentRef</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>outputId</t>
+          <t>parameters</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>valueSource</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>sublist</t>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>reason</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>documentRefs</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>categoryIds</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dataset</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>analysisSetId</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>dataSubsetId</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>orderedGroupings</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>methodId</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>referencedAnalysisOperations</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>programmingCode</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>results</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>controlledTerm</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sponsorTermId</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>context</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>code</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>documentRef</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>parameters</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>valueSource</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>reason</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>purpose</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>documentRefs</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>categoryIds</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>dataset</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>analysisSetId</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>dataSubsetId</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>orderedGroupings</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>methodId</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>referencedAnalysisOperations</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>programmingCode</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>results</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1813,7 +1885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1844,7 +1916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1880,7 +1952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1911,7 +1983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1947,7 +2019,68 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>analysisId</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>outputId</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sublist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1978,7 +2111,130 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>context</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>documentRef</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>parameters</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>operationId</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>resultGroups</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rawValue</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>formattedValue</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1995,160 +2251,6 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>context</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>code</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>documentRef</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>parameters</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>operationId</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>resultGroups</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rawValue</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>formattedValue</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>groupingId</t>
         </is>
       </c>
@@ -2168,7 +2270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2197,14 +2299,14 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"Title,Footnote,Abbreviation,Legend,Rowlabel Header"</formula1>
+      <formula1>"Header,Title,Rowlabel Header,Legend,Abbreviation,Footnote,Footer"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2235,13 +2337,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2290,19 +2392,29 @@
           <t>name</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2331,13 +2443,23 @@
           <t>name</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2373,7 +2495,53 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2404,7 +2572,202 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>display</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>displayTitle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>displaySections</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sectionType</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orderedSubSections</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Header,Title,Rowlabel Header,Legend,Abbreviation,Footnote,Footer"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>subSection</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>subSectionId</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>order</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>subSection</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>subSectionId</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2445,44 +2808,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>display</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2498,67 +2830,21 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>displayTitle</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>displaySections</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sectionType</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>orderedSubSections</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"Title,Footnote,Abbreviation,Legend,Rowlabel Header"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>submissionValue</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2575,26 +2861,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>subSection</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>subSectionId</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>categories</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2611,124 +2897,16 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>subSection</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>subSectionId</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>submissionValue</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>label</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>categories</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>subCategorizations</t>
         </is>
       </c>
@@ -2736,45 +2914,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>condition</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>compoundExpression</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>